<commit_message>
update on parameters in individual age group ideal scenarios
</commit_message>
<xml_diff>
--- a/Ethiopia Workspace/AHLE scenario parameters_examples_WT_GC_complete.xlsx
+++ b/Ethiopia Workspace/AHLE scenario parameters_examples_WT_GC_complete.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gemmachaters/Dropbox/GBADS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gemmachaters/Dropbox/Mac/Documents/GitHub/GBADsLiverpool/Ethiopia Workspace/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5A4753-6DFF-904F-9295-74ACF264C507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3063404B-0ECD-7F4A-94DA-AC391283B85F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="500" windowWidth="19620" windowHeight="15800" xr2:uid="{7B09E95E-6D5F-461A-A5DC-5B71F2D22658}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="361">
   <si>
     <t># Initial population</t>
   </si>
@@ -1577,9 +1577,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDE79AB-593E-49D8-BC0E-644D5608E970}">
   <dimension ref="A1:BB120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="57" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AR1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BA14" sqref="BA14:BA15"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="57" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F124" sqref="F124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11358,23 +11358,23 @@
       <c r="I108">
         <v>1</v>
       </c>
-      <c r="J108" s="20">
-        <v>0.86</v>
-      </c>
-      <c r="K108" s="20">
-        <v>0.86</v>
-      </c>
-      <c r="L108" s="20">
-        <v>0.86</v>
-      </c>
-      <c r="M108" s="20">
-        <v>0.86</v>
-      </c>
-      <c r="N108" s="20">
-        <v>0.86</v>
-      </c>
-      <c r="O108" s="20">
-        <v>0.86</v>
+      <c r="J108">
+        <v>1</v>
+      </c>
+      <c r="K108">
+        <v>1</v>
+      </c>
+      <c r="L108">
+        <v>1</v>
+      </c>
+      <c r="M108">
+        <v>1</v>
+      </c>
+      <c r="N108">
+        <v>1</v>
+      </c>
+      <c r="O108">
+        <v>1</v>
       </c>
       <c r="P108" s="4">
         <v>1</v>
@@ -11397,23 +11397,23 @@
       <c r="V108" s="15">
         <v>1</v>
       </c>
-      <c r="W108" s="18">
-        <v>0.86</v>
-      </c>
-      <c r="X108" s="18">
-        <v>0.86</v>
-      </c>
-      <c r="Y108" s="18">
-        <v>0.86</v>
-      </c>
-      <c r="Z108" s="18">
-        <v>0.86</v>
-      </c>
-      <c r="AA108" s="18">
-        <v>0.86</v>
-      </c>
-      <c r="AB108" s="18">
-        <v>0.86</v>
+      <c r="W108" s="15">
+        <v>1</v>
+      </c>
+      <c r="X108" s="15">
+        <v>1</v>
+      </c>
+      <c r="Y108" s="15">
+        <v>1</v>
+      </c>
+      <c r="Z108" s="15">
+        <v>1</v>
+      </c>
+      <c r="AA108" s="15">
+        <v>1</v>
+      </c>
+      <c r="AB108" s="15">
+        <v>1</v>
       </c>
       <c r="AC108" s="23">
         <v>1</v>
@@ -11436,23 +11436,23 @@
       <c r="AI108">
         <v>1</v>
       </c>
-      <c r="AJ108" s="20">
-        <v>0.86</v>
-      </c>
-      <c r="AK108" s="20">
-        <v>0.86</v>
-      </c>
-      <c r="AL108" s="20">
-        <v>0.86</v>
-      </c>
-      <c r="AM108" s="20">
-        <v>0.86</v>
-      </c>
-      <c r="AN108" s="20">
-        <v>0.86</v>
-      </c>
-      <c r="AO108" s="20">
-        <v>0.86</v>
+      <c r="AJ108">
+        <v>1</v>
+      </c>
+      <c r="AK108">
+        <v>1</v>
+      </c>
+      <c r="AL108">
+        <v>1</v>
+      </c>
+      <c r="AM108">
+        <v>1</v>
+      </c>
+      <c r="AN108">
+        <v>1</v>
+      </c>
+      <c r="AO108">
+        <v>1</v>
       </c>
       <c r="AP108" s="22">
         <v>1</v>
@@ -11475,23 +11475,23 @@
       <c r="AV108" s="8">
         <v>1</v>
       </c>
-      <c r="AW108" s="20">
-        <v>0.86</v>
-      </c>
-      <c r="AX108" s="20">
-        <v>0.86</v>
-      </c>
-      <c r="AY108" s="20">
-        <v>0.86</v>
-      </c>
-      <c r="AZ108" s="20">
-        <v>0.86</v>
-      </c>
-      <c r="BA108" s="20">
-        <v>0.86</v>
-      </c>
-      <c r="BB108" s="20">
-        <v>0.86</v>
+      <c r="AW108" s="8">
+        <v>1</v>
+      </c>
+      <c r="AX108" s="8">
+        <v>1</v>
+      </c>
+      <c r="AY108" s="8">
+        <v>1</v>
+      </c>
+      <c r="AZ108" s="8">
+        <v>1</v>
+      </c>
+      <c r="BA108" s="8">
+        <v>1</v>
+      </c>
+      <c r="BB108" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:54" x14ac:dyDescent="0.2">
@@ -11609,23 +11609,23 @@
       <c r="I114" t="s">
         <v>179</v>
       </c>
-      <c r="J114" s="6">
-        <v>0</v>
-      </c>
-      <c r="K114" s="6">
-        <v>0</v>
-      </c>
-      <c r="L114" s="6">
-        <v>0</v>
-      </c>
-      <c r="M114" s="6">
-        <v>0</v>
-      </c>
-      <c r="N114" s="6">
-        <v>0</v>
-      </c>
-      <c r="O114" s="6">
-        <v>0</v>
+      <c r="J114" t="s">
+        <v>179</v>
+      </c>
+      <c r="K114" t="s">
+        <v>179</v>
+      </c>
+      <c r="L114" t="s">
+        <v>179</v>
+      </c>
+      <c r="M114" t="s">
+        <v>179</v>
+      </c>
+      <c r="N114" t="s">
+        <v>179</v>
+      </c>
+      <c r="O114" t="s">
+        <v>179</v>
       </c>
       <c r="P114" s="4" t="s">
         <v>179</v>
@@ -11648,23 +11648,23 @@
       <c r="V114" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="W114" s="18">
-        <v>0</v>
-      </c>
-      <c r="X114" s="18">
-        <v>0</v>
-      </c>
-      <c r="Y114" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z114" s="18">
-        <v>0</v>
-      </c>
-      <c r="AA114" s="18">
-        <v>0</v>
-      </c>
-      <c r="AB114" s="18">
-        <v>0</v>
+      <c r="W114" t="s">
+        <v>179</v>
+      </c>
+      <c r="X114" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y114" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z114" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA114" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB114" t="s">
+        <v>179</v>
       </c>
       <c r="AC114" t="s">
         <v>179</v>
@@ -11687,23 +11687,23 @@
       <c r="AI114" t="s">
         <v>179</v>
       </c>
-      <c r="AJ114" s="20">
-        <v>0</v>
-      </c>
-      <c r="AK114" s="20">
-        <v>0</v>
-      </c>
-      <c r="AL114" s="20">
-        <v>0</v>
-      </c>
-      <c r="AM114" s="20">
-        <v>0</v>
-      </c>
-      <c r="AN114" s="20">
-        <v>0</v>
-      </c>
-      <c r="AO114" s="20">
-        <v>0</v>
+      <c r="AJ114" t="s">
+        <v>179</v>
+      </c>
+      <c r="AK114" t="s">
+        <v>179</v>
+      </c>
+      <c r="AL114" t="s">
+        <v>179</v>
+      </c>
+      <c r="AM114" t="s">
+        <v>179</v>
+      </c>
+      <c r="AN114" t="s">
+        <v>179</v>
+      </c>
+      <c r="AO114" t="s">
+        <v>179</v>
       </c>
       <c r="AP114" s="22" t="s">
         <v>179</v>
@@ -11726,23 +11726,23 @@
       <c r="AV114" t="s">
         <v>179</v>
       </c>
-      <c r="AW114" s="20">
-        <v>0</v>
-      </c>
-      <c r="AX114" s="20">
-        <v>0</v>
-      </c>
-      <c r="AY114" s="20">
-        <v>0</v>
-      </c>
-      <c r="AZ114" s="20">
-        <v>0</v>
-      </c>
-      <c r="BA114" s="20">
-        <v>0</v>
-      </c>
-      <c r="BB114" s="20">
-        <v>0</v>
+      <c r="AW114" t="s">
+        <v>179</v>
+      </c>
+      <c r="AX114" t="s">
+        <v>179</v>
+      </c>
+      <c r="AY114" t="s">
+        <v>179</v>
+      </c>
+      <c r="AZ114" t="s">
+        <v>179</v>
+      </c>
+      <c r="BA114" t="s">
+        <v>179</v>
+      </c>
+      <c r="BB114" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="115" spans="1:54" x14ac:dyDescent="0.2">

</xml_diff>